<commit_message>
salvado 12 de dic del 2022
</commit_message>
<xml_diff>
--- a/categoria2022.xlsx
+++ b/categoria2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ticom3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2031584A-226E-47C2-83AC-902B9A692970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA57D04F-1D13-44B5-AE26-EBF5B2F40220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="categoria2022" sheetId="1" r:id="rId1"/>
@@ -3473,7 +3473,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4310,17 +4310,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J819"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B781" workbookViewId="0">
       <selection activeCell="G462" sqref="G462:G819"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="36.5703125" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" customWidth="1"/>
     <col min="7" max="7" width="27.7109375" customWidth="1"/>
     <col min="8" max="10" width="36.5703125" customWidth="1"/>
@@ -10022,7 +10023,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" ht="345" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>251</v>
       </c>
@@ -12550,7 +12551,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>335</v>
       </c>
@@ -13958,7 +13959,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>384</v>
       </c>
@@ -17574,7 +17575,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:10" ht="285" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>502</v>
       </c>
@@ -17606,7 +17607,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>504</v>
       </c>
@@ -17670,7 +17671,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>508</v>
       </c>
@@ -17990,7 +17991,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>524</v>
       </c>
@@ -18086,7 +18087,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>528</v>
       </c>
@@ -18118,7 +18119,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>530</v>
       </c>
@@ -18214,7 +18215,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>536</v>
       </c>
@@ -18246,7 +18247,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>538</v>
       </c>
@@ -19078,7 +19079,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="462" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:10" ht="300" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>565</v>
       </c>
@@ -19110,7 +19111,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="463" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:10" ht="210" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>567</v>
       </c>
@@ -19174,7 +19175,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="465" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>570</v>
       </c>
@@ -19270,7 +19271,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="468" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:10" ht="240" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>574</v>
       </c>
@@ -19302,7 +19303,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="469" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:10" ht="345" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>576</v>
       </c>
@@ -19526,7 +19527,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="476" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>585</v>
       </c>
@@ -19654,7 +19655,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="480" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>590</v>
       </c>
@@ -19942,7 +19943,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="489" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>600</v>
       </c>
@@ -20006,7 +20007,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="491" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:10" ht="180" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>603</v>
       </c>
@@ -20038,7 +20039,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="492" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:10" ht="150" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>605</v>
       </c>
@@ -22758,7 +22759,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="577" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
         <v>695</v>
       </c>
@@ -22854,7 +22855,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="580" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:10" ht="270" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
         <v>700</v>
       </c>
@@ -22886,7 +22887,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="581" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:10" ht="195" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
         <v>702</v>
       </c>
@@ -23814,7 +23815,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="610" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
         <v>734</v>
       </c>
@@ -24070,7 +24071,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="618" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:10" ht="120" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
         <v>750</v>
       </c>
@@ -24198,7 +24199,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="622" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="622" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A622" t="s">
         <v>758</v>
       </c>
@@ -25894,7 +25895,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="675" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A675" t="s">
         <v>849</v>
       </c>
@@ -27046,7 +27047,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="711" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="711" spans="1:10" ht="135" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
         <v>921</v>
       </c>
@@ -27654,7 +27655,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="730" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="730" spans="1:10" ht="330" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
         <v>959</v>
       </c>

</xml_diff>